<commit_message>
add column fullname category
</commit_message>
<xml_diff>
--- a/public/assets/template/category-template.xlsx
+++ b/public/assets/template/category-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fitrailyasa\Documents\GitHub\tokusatsu\public\assets\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndejo\Documents\GitHub\tokusatsu\public\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B441176-1848-481E-88D8-4B8DF5CB3164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9FDD05-2A3B-4C5E-8C77-EBD8AC5D91A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{51F6D04B-38A7-4907-901E-8D2AF0D93E74}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{51F6D04B-38A7-4907-901E-8D2AF0D93E74}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Showa</t>
+  </si>
+  <si>
+    <t>Fullname</t>
   </si>
 </sst>
 </file>
@@ -465,24 +468,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86521A1-DC6B-4F40-AA0D-147BEF52CF9B}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="3.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -490,28 +494,32 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -519,21 +527,24 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>